<commit_message>
remove old average code
</commit_message>
<xml_diff>
--- a/storage/excel/sum912.xlsx
+++ b/storage/excel/sum912.xlsx
@@ -2210,24 +2210,12 @@
       <c r="D13" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="89">
-        <v>125282</v>
-      </c>
-      <c r="F13" s="89">
-        <v>8.86</v>
-      </c>
-      <c r="G13" s="89">
-        <v>289165</v>
-      </c>
-      <c r="H13" s="89">
-        <v>9.47</v>
-      </c>
-      <c r="I13" s="89">
-        <v>409454.35528821</v>
-      </c>
-      <c r="J13" s="89">
-        <v>9.17</v>
-      </c>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
       <c r="K13" s="30"/>
       <c r="L13" s="30"/>
       <c r="M13" s="30"/>
@@ -2356,24 +2344,12 @@
       <c r="D14" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="89">
-        <v>540823</v>
-      </c>
-      <c r="F14" s="89">
-        <v>38.25</v>
-      </c>
-      <c r="G14" s="89">
-        <v>772306</v>
-      </c>
-      <c r="H14" s="89">
-        <v>25.29</v>
-      </c>
-      <c r="I14" s="89">
-        <v>1419368.3078626</v>
-      </c>
-      <c r="J14" s="89">
-        <v>31.77</v>
-      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
       <c r="K14" s="30"/>
       <c r="L14" s="30"/>
       <c r="M14" s="30"/>
@@ -2490,24 +2466,12 @@
       <c r="D15" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="89">
-        <v>31734</v>
-      </c>
-      <c r="F15" s="89">
-        <v>2.24</v>
-      </c>
-      <c r="G15" s="89">
-        <v>32329</v>
-      </c>
-      <c r="H15" s="89">
-        <v>1.06</v>
-      </c>
-      <c r="I15" s="89">
-        <v>73783.847510385</v>
-      </c>
-      <c r="J15" s="89">
-        <v>1.65</v>
-      </c>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
       <c r="M15" s="30"/>
@@ -2626,24 +2590,12 @@
       <c r="D16" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="89">
-        <v>54776</v>
-      </c>
-      <c r="F16" s="89">
-        <v>3.87</v>
-      </c>
-      <c r="G16" s="89">
-        <v>163441</v>
-      </c>
-      <c r="H16" s="89">
-        <v>5.35</v>
-      </c>
-      <c r="I16" s="89">
-        <v>206097.01135813</v>
-      </c>
-      <c r="J16" s="89">
-        <v>4.61</v>
-      </c>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
       <c r="K16" s="30"/>
       <c r="L16" s="30"/>
       <c r="M16" s="30"/>
@@ -2766,24 +2718,12 @@
       <c r="D17" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="89">
-        <v>431094</v>
-      </c>
-      <c r="F17" s="89">
-        <v>30.49</v>
-      </c>
-      <c r="G17" s="89">
-        <v>914194</v>
-      </c>
-      <c r="H17" s="89">
-        <v>29.94</v>
-      </c>
-      <c r="I17" s="89">
-        <v>1349807.1786769</v>
-      </c>
-      <c r="J17" s="89">
-        <v>30.22</v>
-      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
       <c r="K17" s="30"/>
       <c r="L17" s="30"/>
       <c r="M17" s="30"/>
@@ -2902,24 +2842,12 @@
       <c r="D18" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="89">
-        <v>5282</v>
-      </c>
-      <c r="F18" s="89">
-        <v>0.37</v>
-      </c>
-      <c r="G18" s="89">
-        <v>12572</v>
-      </c>
-      <c r="H18" s="89">
-        <v>0.41</v>
-      </c>
-      <c r="I18" s="89">
-        <v>17541.334531261</v>
-      </c>
-      <c r="J18" s="89">
-        <v>0.39</v>
-      </c>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
       <c r="M18" s="30"/>
@@ -3042,24 +2970,12 @@
       <c r="D19" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="89">
-        <v>37134</v>
-      </c>
-      <c r="F19" s="89">
-        <v>2.63</v>
-      </c>
-      <c r="G19" s="89">
-        <v>28736</v>
-      </c>
-      <c r="H19" s="89">
-        <v>0.94</v>
-      </c>
-      <c r="I19" s="89">
-        <v>79686.655097893</v>
-      </c>
-      <c r="J19" s="89">
-        <v>1.78</v>
-      </c>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
       <c r="M19" s="30"/>
@@ -3180,24 +3096,12 @@
       <c r="D20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="89">
-        <v>10643</v>
-      </c>
-      <c r="F20" s="89">
-        <v>0.75</v>
-      </c>
-      <c r="G20" s="89">
-        <v>7184</v>
-      </c>
-      <c r="H20" s="89">
-        <v>0.24</v>
-      </c>
-      <c r="I20" s="89">
-        <v>22069.457969833</v>
-      </c>
-      <c r="J20" s="89">
-        <v>0.49</v>
-      </c>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
       <c r="K20" s="30"/>
       <c r="L20" s="30"/>
       <c r="M20" s="30"/>
@@ -3328,24 +3232,12 @@
       <c r="D21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="89">
-        <v>14132</v>
-      </c>
-      <c r="F21" s="89">
-        <v>1</v>
-      </c>
-      <c r="G21" s="89">
-        <v>16164</v>
-      </c>
-      <c r="H21" s="89">
-        <v>0.53</v>
-      </c>
-      <c r="I21" s="89">
-        <v>34150.533408288</v>
-      </c>
-      <c r="J21" s="89">
-        <v>0.76</v>
-      </c>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
       <c r="M21" s="30"/>
@@ -3470,24 +3362,12 @@
       <c r="D22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="89">
-        <v>12378</v>
-      </c>
-      <c r="F22" s="89">
-        <v>0.88</v>
-      </c>
-      <c r="G22" s="89">
-        <v>16164</v>
-      </c>
-      <c r="H22" s="89">
-        <v>0.53</v>
-      </c>
-      <c r="I22" s="89">
-        <v>31379.491835166</v>
-      </c>
-      <c r="J22" s="89">
-        <v>0.7</v>
-      </c>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
       <c r="K22" s="30"/>
       <c r="L22" s="30"/>
       <c r="M22" s="30"/>
@@ -3614,24 +3494,12 @@
       <c r="D23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="89">
-        <v>334195</v>
-      </c>
-      <c r="F23" s="89">
-        <v>23.64</v>
-      </c>
-      <c r="G23" s="89">
-        <v>213731</v>
-      </c>
-      <c r="H23" s="89">
-        <v>7</v>
-      </c>
-      <c r="I23" s="89">
-        <v>684322.5918548</v>
-      </c>
-      <c r="J23" s="89">
-        <v>15.32</v>
-      </c>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
       <c r="M23" s="30"/>
@@ -3764,24 +3632,12 @@
       <c r="D24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="89">
-        <v>33626</v>
-      </c>
-      <c r="F24" s="89">
-        <v>2.38</v>
-      </c>
-      <c r="G24" s="89">
-        <v>19756</v>
-      </c>
-      <c r="H24" s="89">
-        <v>0.65</v>
-      </c>
-      <c r="I24" s="89">
-        <v>67575.562675463</v>
-      </c>
-      <c r="J24" s="89">
-        <v>1.51</v>
-      </c>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
       <c r="K24" s="30"/>
       <c r="L24" s="30"/>
       <c r="M24" s="30"/>
@@ -3914,24 +3770,12 @@
       <c r="D25" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="89">
-        <v>206667</v>
-      </c>
-      <c r="F25" s="89">
-        <v>14.62</v>
-      </c>
-      <c r="G25" s="89">
-        <v>440034</v>
-      </c>
-      <c r="H25" s="89">
-        <v>14.41</v>
-      </c>
-      <c r="I25" s="89">
-        <v>648392.74979379</v>
-      </c>
-      <c r="J25" s="89">
-        <v>14.51</v>
-      </c>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="30"/>
       <c r="K25" s="30"/>
       <c r="L25" s="30"/>
       <c r="M25" s="30"/>
@@ -4060,24 +3904,12 @@
       <c r="D26" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="89">
-        <v>561796</v>
-      </c>
-      <c r="F26" s="89">
-        <v>39.74</v>
-      </c>
-      <c r="G26" s="89">
-        <v>867497</v>
-      </c>
-      <c r="H26" s="89">
-        <v>28.41</v>
-      </c>
-      <c r="I26" s="89">
-        <v>1522136.0115195</v>
-      </c>
-      <c r="J26" s="89">
-        <v>34.07</v>
-      </c>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
       <c r="K26" s="30"/>
       <c r="L26" s="30"/>
       <c r="M26" s="30"/>
@@ -4198,24 +4030,12 @@
       <c r="D27" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="89">
-        <v>17739</v>
-      </c>
-      <c r="F27" s="89">
-        <v>1.25</v>
-      </c>
-      <c r="G27" s="89">
-        <v>30533</v>
-      </c>
-      <c r="H27" s="89">
-        <v>1</v>
-      </c>
-      <c r="I27" s="89">
-        <v>50360.167196852</v>
-      </c>
-      <c r="J27" s="89">
-        <v>1.13</v>
-      </c>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
       <c r="K27" s="30"/>
       <c r="L27" s="30"/>
       <c r="M27" s="30"/>
@@ -4348,24 +4168,12 @@
       <c r="D28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="89">
-        <v>63665</v>
-      </c>
-      <c r="F28" s="89">
-        <v>4.5</v>
-      </c>
-      <c r="G28" s="89">
-        <v>131112</v>
-      </c>
-      <c r="H28" s="89">
-        <v>4.29</v>
-      </c>
-      <c r="I28" s="89">
-        <v>196491.05542412</v>
-      </c>
-      <c r="J28" s="89">
-        <v>4.4</v>
-      </c>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30"/>
       <c r="K28" s="30"/>
       <c r="L28" s="30"/>
       <c r="M28" s="30"/>
@@ -4498,24 +4306,12 @@
       <c r="D29" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="89">
-        <v>31852</v>
-      </c>
-      <c r="F29" s="89">
-        <v>2.25</v>
-      </c>
-      <c r="G29" s="89">
-        <v>21552</v>
-      </c>
-      <c r="H29" s="89">
-        <v>0.71</v>
-      </c>
-      <c r="I29" s="89">
-        <v>66086.726132342</v>
-      </c>
-      <c r="J29" s="89">
-        <v>1.48</v>
-      </c>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
       <c r="K29" s="30"/>
       <c r="L29" s="30"/>
       <c r="M29" s="30"/>
@@ -4648,24 +4444,12 @@
       <c r="D30" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="89">
-        <v>7095</v>
-      </c>
-      <c r="F30" s="89">
-        <v>0.5</v>
-      </c>
-      <c r="G30" s="89">
-        <v>14368</v>
-      </c>
-      <c r="H30" s="89">
-        <v>0.47</v>
-      </c>
-      <c r="I30" s="89">
-        <v>21719.388594064</v>
-      </c>
-      <c r="J30" s="89">
-        <v>0.49</v>
-      </c>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
       <c r="K30" s="30"/>
       <c r="L30" s="30"/>
       <c r="M30" s="30"/>
@@ -4798,24 +4582,12 @@
       <c r="D31" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="89">
-        <v>3528</v>
-      </c>
-      <c r="F31" s="89">
-        <v>0.25</v>
-      </c>
-      <c r="G31" s="89">
-        <v>8980</v>
-      </c>
-      <c r="H31" s="89">
-        <v>0.29</v>
-      </c>
-      <c r="I31" s="89">
-        <v>12142.689247664</v>
-      </c>
-      <c r="J31" s="89">
-        <v>0.27</v>
-      </c>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
       <c r="K31" s="30"/>
       <c r="L31" s="30"/>
       <c r="M31" s="30"/>
@@ -4948,24 +4720,12 @@
       <c r="D32" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="89">
-        <v>1042757</v>
-      </c>
-      <c r="F32" s="89">
-        <v>73.76</v>
-      </c>
-      <c r="G32" s="89">
-        <v>2227115</v>
-      </c>
-      <c r="H32" s="89">
-        <v>72.94</v>
-      </c>
-      <c r="I32" s="89">
-        <v>3276559.6987433</v>
-      </c>
-      <c r="J32" s="89">
-        <v>73.35</v>
-      </c>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
       <c r="K32" s="30"/>
       <c r="L32" s="30"/>
       <c r="M32" s="30"/>
@@ -5096,24 +4856,12 @@
       <c r="D33" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="89">
-        <v>224348</v>
-      </c>
-      <c r="F33" s="89">
-        <v>15.87</v>
-      </c>
-      <c r="G33" s="89">
-        <v>226303</v>
-      </c>
-      <c r="H33" s="89">
-        <v>7.41</v>
-      </c>
-      <c r="I33" s="89">
-        <v>519978.38176118</v>
-      </c>
-      <c r="J33" s="89">
-        <v>11.64</v>
-      </c>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
       <c r="K33" s="30"/>
       <c r="L33" s="30"/>
       <c r="M33" s="30"/>
@@ -5238,24 +4986,12 @@
       <c r="D34" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="89">
-        <v>115050</v>
-      </c>
-      <c r="F34" s="89">
-        <v>8.14</v>
-      </c>
-      <c r="G34" s="89">
-        <v>154461</v>
-      </c>
-      <c r="H34" s="89">
-        <v>5.06</v>
-      </c>
-      <c r="I34" s="89">
-        <v>294751.35429311</v>
-      </c>
-      <c r="J34" s="89">
-        <v>6.6</v>
-      </c>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
       <c r="K34" s="30"/>
       <c r="L34" s="30"/>
       <c r="M34" s="30"/>
@@ -5382,24 +5118,12 @@
       <c r="D35" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="89">
-        <v>1773</v>
-      </c>
-      <c r="F35" s="89">
-        <v>0.13</v>
-      </c>
-      <c r="G35" s="89">
-        <v>1796</v>
-      </c>
-      <c r="H35" s="89">
-        <v>0.06</v>
-      </c>
-      <c r="I35" s="89">
-        <v>4114.8604123329</v>
-      </c>
-      <c r="J35" s="89">
-        <v>0.09</v>
-      </c>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
       <c r="K35" s="30"/>
       <c r="L35" s="30"/>
       <c r="M35" s="30"/>
@@ -5530,24 +5254,12 @@
       <c r="D36" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="89">
-        <v>8830</v>
-      </c>
-      <c r="F36" s="89">
-        <v>0.62</v>
-      </c>
-      <c r="G36" s="89">
-        <v>8980</v>
-      </c>
-      <c r="H36" s="89">
-        <v>0.29</v>
-      </c>
-      <c r="I36" s="89">
-        <v>20519.007617503</v>
-      </c>
-      <c r="J36" s="89">
-        <v>0.46</v>
-      </c>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
       <c r="K36" s="30"/>
       <c r="L36" s="30"/>
       <c r="M36" s="30"/>
@@ -5673,24 +5385,12 @@
       <c r="D37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="89">
-        <v>0</v>
-      </c>
-      <c r="F37" s="89">
-        <v>0</v>
-      </c>
-      <c r="G37" s="89">
-        <v>0</v>
-      </c>
-      <c r="H37" s="89">
-        <v>0</v>
-      </c>
-      <c r="I37" s="89">
-        <v>0</v>
-      </c>
-      <c r="J37" s="89">
-        <v>0</v>
-      </c>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
       <c r="K37" s="30"/>
       <c r="L37" s="30"/>
       <c r="M37" s="30"/>
@@ -5816,24 +5516,12 @@
       <c r="D38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E38" s="89">
-        <v>0</v>
-      </c>
-      <c r="F38" s="89">
-        <v>0</v>
-      </c>
-      <c r="G38" s="89">
-        <v>0</v>
-      </c>
-      <c r="H38" s="89">
-        <v>0</v>
-      </c>
-      <c r="I38" s="89">
-        <v>0</v>
-      </c>
-      <c r="J38" s="89">
-        <v>0</v>
-      </c>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
       <c r="K38" s="30"/>
       <c r="L38" s="30"/>
       <c r="M38" s="30"/>
@@ -5961,24 +5649,12 @@
       <c r="D39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="89">
-        <v>182440</v>
-      </c>
-      <c r="F39" s="89">
-        <v>12.9</v>
-      </c>
-      <c r="G39" s="89">
-        <v>827983</v>
-      </c>
-      <c r="H39" s="89">
-        <v>27.12</v>
-      </c>
-      <c r="I39" s="89">
-        <v>893908.64597796</v>
-      </c>
-      <c r="J39" s="89">
-        <v>20.01</v>
-      </c>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
       <c r="K39" s="30"/>
       <c r="L39" s="30"/>
       <c r="M39" s="30"/>
@@ -6110,24 +5786,12 @@
       <c r="D40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="89">
-        <v>434465</v>
-      </c>
-      <c r="F40" s="89">
-        <v>30.73</v>
-      </c>
-      <c r="G40" s="89">
-        <v>1311124</v>
-      </c>
-      <c r="H40" s="89">
-        <v>42.94</v>
-      </c>
-      <c r="I40" s="89">
-        <v>1645493.2747948</v>
-      </c>
-      <c r="J40" s="89">
-        <v>36.84</v>
-      </c>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
       <c r="K40" s="30"/>
       <c r="L40" s="30"/>
       <c r="M40" s="30"/>
@@ -6253,24 +5917,12 @@
       <c r="D41" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E41" s="89">
-        <v>1773</v>
-      </c>
-      <c r="F41" s="89">
-        <v>0.13</v>
-      </c>
-      <c r="G41" s="89">
-        <v>0</v>
-      </c>
-      <c r="H41" s="89">
-        <v>0</v>
-      </c>
-      <c r="I41" s="89">
-        <v>2801.0585570961</v>
-      </c>
-      <c r="J41" s="89">
-        <v>0.06</v>
-      </c>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
       <c r="K41" s="30"/>
       <c r="L41" s="30"/>
       <c r="M41" s="30"/>
@@ -6395,24 +6047,12 @@
       <c r="D42" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="89">
-        <v>1773</v>
-      </c>
-      <c r="F42" s="89">
-        <v>0.13</v>
-      </c>
-      <c r="G42" s="89">
-        <v>0</v>
-      </c>
-      <c r="H42" s="89">
-        <v>0</v>
-      </c>
-      <c r="I42" s="89">
-        <v>2801.0585570961</v>
-      </c>
-      <c r="J42" s="89">
-        <v>0.06</v>
-      </c>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
       <c r="K42" s="30"/>
       <c r="L42" s="30"/>
       <c r="M42" s="30"/>
@@ -6539,24 +6179,12 @@
       <c r="D43" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E43" s="89">
-        <v>10584</v>
-      </c>
-      <c r="F43" s="89">
-        <v>0.75</v>
-      </c>
-      <c r="G43" s="89">
-        <v>50289</v>
-      </c>
-      <c r="H43" s="89">
-        <v>1.65</v>
-      </c>
-      <c r="I43" s="89">
-        <v>53508.223376581</v>
-      </c>
-      <c r="J43" s="89">
-        <v>1.2</v>
-      </c>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
       <c r="K43" s="30"/>
       <c r="L43" s="30"/>
       <c r="M43" s="30"/>
@@ -6687,24 +6315,12 @@
       <c r="D44" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="89">
-        <v>24697</v>
-      </c>
-      <c r="F44" s="89">
-        <v>1.75</v>
-      </c>
-      <c r="G44" s="89">
-        <v>109559</v>
-      </c>
-      <c r="H44" s="89">
-        <v>3.59</v>
-      </c>
-      <c r="I44" s="89">
-        <v>119161.4473576</v>
-      </c>
-      <c r="J44" s="89">
-        <v>2.67</v>
-      </c>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
       <c r="K44" s="30"/>
       <c r="L44" s="30"/>
       <c r="M44" s="30"/>
@@ -6829,24 +6445,12 @@
       <c r="D45" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E45" s="89">
-        <v>0</v>
-      </c>
-      <c r="F45" s="89">
-        <v>0</v>
-      </c>
-      <c r="G45" s="89">
-        <v>0</v>
-      </c>
-      <c r="H45" s="89">
-        <v>0</v>
-      </c>
-      <c r="I45" s="89">
-        <v>0</v>
-      </c>
-      <c r="J45" s="89">
-        <v>0</v>
-      </c>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
       <c r="K45" s="30"/>
       <c r="L45" s="30"/>
       <c r="M45" s="30"/>
@@ -6971,24 +6575,12 @@
       <c r="D46" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E46" s="89">
-        <v>0</v>
-      </c>
-      <c r="F46" s="89">
-        <v>0</v>
-      </c>
-      <c r="G46" s="89">
-        <v>0</v>
-      </c>
-      <c r="H46" s="89">
-        <v>0</v>
-      </c>
-      <c r="I46" s="89">
-        <v>0</v>
-      </c>
-      <c r="J46" s="89">
-        <v>0</v>
-      </c>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
       <c r="K46" s="30"/>
       <c r="L46" s="30"/>
       <c r="M46" s="30"/>
@@ -7115,24 +6707,12 @@
       <c r="D47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E47" s="89">
-        <v>1754</v>
-      </c>
-      <c r="F47" s="89">
-        <v>0.12</v>
-      </c>
-      <c r="G47" s="89">
-        <v>48493</v>
-      </c>
-      <c r="H47" s="89">
-        <v>1.59</v>
-      </c>
-      <c r="I47" s="89">
-        <v>38244.423180025</v>
-      </c>
-      <c r="J47" s="89">
-        <v>0.86</v>
-      </c>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
       <c r="K47" s="30"/>
       <c r="L47" s="30"/>
       <c r="M47" s="30"/>
@@ -7263,24 +6843,12 @@
       <c r="D48" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E48" s="89">
-        <v>5262</v>
-      </c>
-      <c r="F48" s="89">
-        <v>0.37</v>
-      </c>
-      <c r="G48" s="89">
-        <v>10776</v>
-      </c>
-      <c r="H48" s="89">
-        <v>0.35</v>
-      </c>
-      <c r="I48" s="89">
-        <v>16195.935850789</v>
-      </c>
-      <c r="J48" s="89">
-        <v>0.36</v>
-      </c>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
       <c r="K48" s="30"/>
       <c r="L48" s="30"/>
       <c r="M48" s="30"/>
@@ -7405,24 +6973,12 @@
       <c r="D49" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E49" s="89">
-        <v>0</v>
-      </c>
-      <c r="F49" s="89">
-        <v>0</v>
-      </c>
-      <c r="G49" s="89">
-        <v>0</v>
-      </c>
-      <c r="H49" s="89">
-        <v>0</v>
-      </c>
-      <c r="I49" s="89">
-        <v>0</v>
-      </c>
-      <c r="J49" s="89">
-        <v>0</v>
-      </c>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="30"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="30"/>
       <c r="K49" s="30"/>
       <c r="L49" s="30"/>
       <c r="M49" s="30"/>
@@ -7547,24 +7103,12 @@
       <c r="D50" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E50" s="89">
-        <v>0</v>
-      </c>
-      <c r="F50" s="89">
-        <v>0</v>
-      </c>
-      <c r="G50" s="89">
-        <v>1796</v>
-      </c>
-      <c r="H50" s="89">
-        <v>0.06</v>
-      </c>
-      <c r="I50" s="89">
-        <v>1313.8018552368</v>
-      </c>
-      <c r="J50" s="89">
-        <v>0.03</v>
-      </c>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="30"/>
       <c r="K50" s="30"/>
       <c r="L50" s="30"/>
       <c r="M50" s="30"/>
@@ -7691,24 +7235,12 @@
       <c r="D51" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E51" s="89">
-        <v>1754</v>
-      </c>
-      <c r="F51" s="89">
-        <v>0.12</v>
-      </c>
-      <c r="G51" s="89">
-        <v>35921</v>
-      </c>
-      <c r="H51" s="89">
-        <v>1.18</v>
-      </c>
-      <c r="I51" s="89">
-        <v>29047.810193368</v>
-      </c>
-      <c r="J51" s="89">
-        <v>0.65</v>
-      </c>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="30"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="30"/>
+      <c r="J51" s="30"/>
       <c r="K51" s="30"/>
       <c r="L51" s="30"/>
       <c r="M51" s="30"/>
@@ -7839,24 +7371,12 @@
       <c r="D52" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E52" s="89">
-        <v>3547</v>
-      </c>
-      <c r="F52" s="89">
-        <v>0.25</v>
-      </c>
-      <c r="G52" s="89">
-        <v>5388</v>
-      </c>
-      <c r="H52" s="89">
-        <v>0.18</v>
-      </c>
-      <c r="I52" s="89">
-        <v>9545.1025211643</v>
-      </c>
-      <c r="J52" s="89">
-        <v>0.21</v>
-      </c>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="30"/>
+      <c r="I52" s="30"/>
+      <c r="J52" s="30"/>
       <c r="K52" s="30"/>
       <c r="L52" s="30"/>
       <c r="M52" s="30"/>
@@ -7981,24 +7501,12 @@
       <c r="D53" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E53" s="89">
-        <v>0</v>
-      </c>
-      <c r="F53" s="89">
-        <v>0</v>
-      </c>
-      <c r="G53" s="89">
-        <v>0</v>
-      </c>
-      <c r="H53" s="89">
-        <v>0</v>
-      </c>
-      <c r="I53" s="89">
-        <v>0</v>
-      </c>
-      <c r="J53" s="89">
-        <v>0</v>
-      </c>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="30"/>
+      <c r="H53" s="30"/>
+      <c r="I53" s="30"/>
+      <c r="J53" s="30"/>
       <c r="K53" s="30"/>
       <c r="L53" s="30"/>
       <c r="M53" s="30"/>
@@ -8123,24 +7631,12 @@
       <c r="D54" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E54" s="89">
-        <v>0</v>
-      </c>
-      <c r="F54" s="89">
-        <v>0</v>
-      </c>
-      <c r="G54" s="89">
-        <v>0</v>
-      </c>
-      <c r="H54" s="89">
-        <v>0</v>
-      </c>
-      <c r="I54" s="89">
-        <v>0</v>
-      </c>
-      <c r="J54" s="89">
-        <v>0</v>
-      </c>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="30"/>
+      <c r="I54" s="30"/>
+      <c r="J54" s="30"/>
       <c r="K54" s="30"/>
       <c r="L54" s="30"/>
       <c r="M54" s="30"/>

</xml_diff>

<commit_message>
change report912 to go to seperate file and change Summary::sum to use settins from database instead of from excel sheets
</commit_message>
<xml_diff>
--- a/storage/excel/sum912.xlsx
+++ b/storage/excel/sum912.xlsx
@@ -2285,19 +2285,19 @@
         <v>7.2529141210443</v>
       </c>
       <c r="AM13" s="89">
-        <v>0.61802081225418</v>
+        <v>0.65276227089399</v>
       </c>
       <c r="AN13" s="89">
         <v>24.360220764856</v>
       </c>
       <c r="AO13" s="89">
-        <v>2.0757344113734</v>
+        <v>2.192419868837</v>
       </c>
       <c r="AP13" s="89">
         <v>31.364880132893</v>
       </c>
       <c r="AQ13" s="89">
-        <v>2.6726014361239</v>
+        <v>2.8228392119604</v>
       </c>
       <c r="AR13" s="30"/>
       <c r="AS13" s="30"/>
@@ -2423,19 +2423,19 @@
         <v>55.165727229407</v>
       </c>
       <c r="AM14" s="89">
-        <v>4.7006716172178</v>
+        <v>4.9649154506467</v>
       </c>
       <c r="AN14" s="89">
         <v>86.749308557244</v>
       </c>
       <c r="AO14" s="89">
-        <v>7.3919085821628</v>
+        <v>7.807437770152</v>
       </c>
       <c r="AP14" s="89">
         <v>142.83971896297</v>
       </c>
       <c r="AQ14" s="89">
-        <v>12.171372452835</v>
+        <v>12.855574706667</v>
       </c>
       <c r="AR14" s="30"/>
       <c r="AS14" s="30"/>
@@ -2557,19 +2557,19 @@
         <v>6.8460990093975</v>
       </c>
       <c r="AM15" s="89">
-        <v>0.58335609659076</v>
+        <v>0.61614891084578</v>
       </c>
       <c r="AN15" s="89">
         <v>7.184322960601</v>
       </c>
       <c r="AO15" s="89">
-        <v>0.61217615947281</v>
+        <v>0.64658906645409</v>
       </c>
       <c r="AP15" s="89">
         <v>14.247412992399</v>
       </c>
       <c r="AQ15" s="89">
-        <v>1.2140220610823</v>
+        <v>1.2822671693159</v>
       </c>
       <c r="AR15" s="30"/>
       <c r="AS15" s="30"/>
@@ -2697,19 +2697,19 @@
         <v>3.2685301642238</v>
       </c>
       <c r="AM16" s="89">
-        <v>0.27851145529351</v>
+        <v>0.29416771478014</v>
       </c>
       <c r="AN16" s="89">
         <v>14.254972421492</v>
       </c>
       <c r="AO16" s="89">
-        <v>1.2146662000353</v>
+        <v>1.2829475179343</v>
       </c>
       <c r="AP16" s="89">
         <v>17.318075901583</v>
       </c>
       <c r="AQ16" s="89">
-        <v>1.4756732475739</v>
+        <v>1.5586268311425</v>
       </c>
       <c r="AR16" s="30"/>
       <c r="AS16" s="30"/>
@@ -2833,19 +2833,19 @@
         <v>53.979867866856</v>
       </c>
       <c r="AM17" s="89">
-        <v>4.5996245409348</v>
+        <v>4.8581881080171</v>
       </c>
       <c r="AN17" s="89">
         <v>112.25588477866</v>
       </c>
       <c r="AO17" s="89">
-        <v>9.5653239419896</v>
+        <v>10.103029630079</v>
       </c>
       <c r="AP17" s="89">
         <v>166.35917712867</v>
       </c>
       <c r="AQ17" s="89">
-        <v>14.175465483134</v>
+        <v>14.97232594158</v>
       </c>
       <c r="AR17" s="30"/>
       <c r="AS17" s="30"/>
@@ -2973,19 +2973,19 @@
         <v>1.0768426722641</v>
       </c>
       <c r="AM18" s="89">
-        <v>0.091757764103621</v>
+        <v>0.096915840503766</v>
       </c>
       <c r="AN18" s="89">
         <v>2.5835317051781</v>
       </c>
       <c r="AO18" s="89">
-        <v>0.22014273659823</v>
+        <v>0.23251785346603</v>
       </c>
       <c r="AP18" s="89">
         <v>3.653012190404</v>
       </c>
       <c r="AQ18" s="89">
-        <v>0.31127316874432</v>
+        <v>0.32877109713636</v>
       </c>
       <c r="AR18" s="30"/>
       <c r="AS18" s="30"/>
@@ -3109,19 +3109,19 @@
         <v>5.7506548997069</v>
       </c>
       <c r="AM19" s="89">
-        <v>0.49001330400402</v>
+        <v>0.51755894097362</v>
       </c>
       <c r="AN19" s="89">
         <v>3.322467096181</v>
       </c>
       <c r="AO19" s="89">
-        <v>0.28310742126559</v>
+        <v>0.29902203865629</v>
       </c>
       <c r="AP19" s="89">
         <v>9.33282120007</v>
       </c>
       <c r="AQ19" s="89">
-        <v>0.79524969445797</v>
+        <v>0.8399539080063</v>
       </c>
       <c r="AR19" s="30"/>
       <c r="AS19" s="30"/>
@@ -3255,19 +3255,19 @@
         <v>3.2377973459364</v>
       </c>
       <c r="AM20" s="89">
-        <v>0.27589271184724</v>
+        <v>0.29140176113428</v>
       </c>
       <c r="AN20" s="89">
         <v>2.3254078683687</v>
       </c>
       <c r="AO20" s="89">
-        <v>0.1981480044637</v>
+        <v>0.20928670815318</v>
       </c>
       <c r="AP20" s="89">
         <v>5.6964418396012</v>
       </c>
       <c r="AQ20" s="89">
-        <v>0.48539380915242</v>
+        <v>0.51267976556411</v>
       </c>
       <c r="AR20" s="30"/>
       <c r="AS20" s="30"/>
@@ -3399,19 +3399,19 @@
         <v>4.5594829810831</v>
       </c>
       <c r="AM21" s="89">
-        <v>0.38851354481809</v>
+        <v>0.41035346829748</v>
       </c>
       <c r="AN21" s="89">
         <v>3.994893802646</v>
       </c>
       <c r="AO21" s="89">
-        <v>0.34040490092347</v>
+        <v>0.35954044223814</v>
       </c>
       <c r="AP21" s="89">
         <v>8.721440238677</v>
       </c>
       <c r="AQ21" s="89">
-        <v>0.74315392273767</v>
+        <v>0.78492962148093</v>
       </c>
       <c r="AR21" s="30"/>
       <c r="AS21" s="30"/>
@@ -3541,19 +3541,19 @@
         <v>68.996380666104</v>
       </c>
       <c r="AM22" s="89">
-        <v>5.8791815965587</v>
+        <v>6.2096742599493</v>
       </c>
       <c r="AN22" s="89">
         <v>5.6993641972234</v>
       </c>
       <c r="AO22" s="89">
-        <v>0.48564282324541</v>
+        <v>0.51294277775011</v>
       </c>
       <c r="AP22" s="89">
         <v>78.786899296487</v>
       </c>
       <c r="AQ22" s="89">
-        <v>6.7134316890537</v>
+        <v>7.0908209366839</v>
       </c>
       <c r="AR22" s="30"/>
       <c r="AS22" s="30"/>
@@ -3689,19 +3689,19 @@
         <v>12.522716619176</v>
       </c>
       <c r="AM23" s="89">
-        <v>1.06706068312</v>
+        <v>1.1270444957259</v>
       </c>
       <c r="AN23" s="89">
         <v>8.3902568407534</v>
       </c>
       <c r="AO23" s="89">
-        <v>0.7149337854006</v>
+        <v>0.75512311566781</v>
       </c>
       <c r="AP23" s="89">
         <v>21.44552056842</v>
       </c>
       <c r="AQ23" s="89">
-        <v>1.827372807635</v>
+        <v>1.9300968511578</v>
       </c>
       <c r="AR23" s="30"/>
       <c r="AS23" s="30"/>
@@ -3839,19 +3839,19 @@
         <v>5.9517726409752</v>
       </c>
       <c r="AM24" s="89">
-        <v>0.5071505467375</v>
+        <v>0.53565953768777</v>
       </c>
       <c r="AN24" s="89">
         <v>2.0696568123669</v>
       </c>
       <c r="AO24" s="89">
-        <v>0.17635545698178</v>
+        <v>0.18626911311302</v>
       </c>
       <c r="AP24" s="89">
         <v>8.3292927159471</v>
       </c>
       <c r="AQ24" s="89">
-        <v>0.70973903232585</v>
+        <v>0.74963634443524</v>
       </c>
       <c r="AR24" s="30"/>
       <c r="AS24" s="30"/>
@@ -3989,19 +3989,19 @@
         <v>13.855609569265</v>
       </c>
       <c r="AM25" s="89">
-        <v>1.180636491397</v>
+        <v>1.2470048612338</v>
       </c>
       <c r="AN25" s="89">
         <v>19.999833528298</v>
       </c>
       <c r="AO25" s="89">
-        <v>1.7041858149463</v>
+        <v>1.7999850175468</v>
       </c>
       <c r="AP25" s="89">
         <v>34.138744224845</v>
       </c>
       <c r="AQ25" s="89">
-        <v>2.9089623953991</v>
+        <v>3.0724869802361</v>
       </c>
       <c r="AR25" s="30"/>
       <c r="AS25" s="30"/>
@@ -4127,19 +4127,19 @@
         <v>53.770353473322</v>
       </c>
       <c r="AM26" s="89">
-        <v>4.5817718194618</v>
+        <v>4.839331812599</v>
       </c>
       <c r="AN26" s="89">
         <v>75.405908066947</v>
       </c>
       <c r="AO26" s="89">
-        <v>6.4253374263845</v>
+        <v>6.7865317260252</v>
       </c>
       <c r="AP26" s="89">
         <v>130.33873990894</v>
       </c>
       <c r="AQ26" s="89">
-        <v>11.10616402764</v>
+        <v>11.730486591804</v>
       </c>
       <c r="AR26" s="30"/>
       <c r="AS26" s="30"/>
@@ -4273,19 +4273,19 @@
         <v>1.2270703161888</v>
       </c>
       <c r="AM27" s="89">
-        <v>0.10455866164245</v>
+        <v>0.11043632845699</v>
       </c>
       <c r="AN27" s="89">
         <v>2.1903999105404</v>
       </c>
       <c r="AO27" s="89">
-        <v>0.18664397637714</v>
+        <v>0.19713599194863</v>
       </c>
       <c r="AP27" s="89">
         <v>3.4305929657554</v>
       </c>
       <c r="AQ27" s="89">
-        <v>0.29232082661202</v>
+        <v>0.30875336691798</v>
       </c>
       <c r="AR27" s="30"/>
       <c r="AS27" s="30"/>
@@ -4423,19 +4423,19 @@
         <v>12.469433584727</v>
       </c>
       <c r="AM28" s="89">
-        <v>1.0625204357546</v>
+        <v>1.1222490226254</v>
       </c>
       <c r="AN28" s="89">
         <v>11.795963235726</v>
       </c>
       <c r="AO28" s="89">
-        <v>1.0051340273162</v>
+        <v>1.0616366912153</v>
       </c>
       <c r="AP28" s="89">
         <v>24.697434778724</v>
       </c>
       <c r="AQ28" s="89">
-        <v>2.104468417495</v>
+        <v>2.2227691300851</v>
       </c>
       <c r="AR28" s="30"/>
       <c r="AS28" s="30"/>
@@ -4573,19 +4573,19 @@
         <v>1.1302823741379</v>
       </c>
       <c r="AM29" s="89">
-        <v>0.096311361100287</v>
+        <v>0.10172541367241</v>
       </c>
       <c r="AN29" s="89">
         <v>1.1581269133533</v>
       </c>
       <c r="AO29" s="89">
-        <v>0.098683994286836</v>
+        <v>0.1042314222018</v>
       </c>
       <c r="AP29" s="89">
         <v>2.325033441309</v>
       </c>
       <c r="AQ29" s="89">
-        <v>0.19811609953394</v>
+        <v>0.20925300971781</v>
       </c>
       <c r="AR29" s="30"/>
       <c r="AS29" s="30"/>
@@ -4723,19 +4723,19 @@
         <v>0.11268266469474</v>
       </c>
       <c r="AM30" s="89">
-        <v>0.0096016898586385</v>
+        <v>0.010141439822526</v>
       </c>
       <c r="AN30" s="89">
         <v>0.94966944525756</v>
       </c>
       <c r="AO30" s="89">
-        <v>0.080921333430396</v>
+        <v>0.08547025007318</v>
       </c>
       <c r="AP30" s="89">
         <v>1.042188774615</v>
       </c>
       <c r="AQ30" s="89">
-        <v>0.088804905484942</v>
+        <v>0.093796989715348</v>
       </c>
       <c r="AR30" s="30"/>
       <c r="AS30" s="30"/>
@@ -4873,19 +4873,19 @@
         <v>0.35155486341358</v>
       </c>
       <c r="AM31" s="89">
-        <v>0.029955989911472</v>
+        <v>0.031639937707223</v>
       </c>
       <c r="AN31" s="89">
         <v>0.78252006551545</v>
       </c>
       <c r="AO31" s="89">
-        <v>0.066678534782572</v>
+        <v>0.070426805896391</v>
       </c>
       <c r="AP31" s="89">
         <v>1.1334105403331</v>
       </c>
       <c r="AQ31" s="89">
-        <v>0.096577912141781</v>
+        <v>0.10200694862998</v>
       </c>
       <c r="AR31" s="30"/>
       <c r="AS31" s="30"/>
@@ -5023,19 +5023,19 @@
         <v>3.3753127043595</v>
       </c>
       <c r="AM32" s="90">
-        <v>3.4831201921367E-5</v>
+        <v>2.8352626716619E-5</v>
       </c>
       <c r="AN32" s="90">
         <v>1.6769520509725</v>
       </c>
       <c r="AO32" s="90">
-        <v>1.7305138994806E-5</v>
+        <v>1.4086397228169E-5</v>
       </c>
       <c r="AP32" s="90">
         <v>5.2124913898245</v>
       </c>
       <c r="AQ32" s="90">
-        <v>5.3789783648155E-5</v>
+        <v>4.3784927674526E-5</v>
       </c>
       <c r="AR32" s="36"/>
       <c r="AS32" s="36"/>
@@ -5167,19 +5167,19 @@
         <v>0.44458062677522</v>
       </c>
       <c r="AM33" s="89">
-        <v>4.5878053199442E-6</v>
+        <v>3.7344772649119E-6</v>
       </c>
       <c r="AN33" s="89">
         <v>0.13241995504941</v>
       </c>
       <c r="AO33" s="89">
-        <v>1.3664944841369E-6</v>
+        <v>1.1123276224151E-6</v>
       </c>
       <c r="AP33" s="89">
         <v>0.60063021112989</v>
       </c>
       <c r="AQ33" s="89">
-        <v>6.1981434007338E-6</v>
+        <v>5.0452937734911E-6</v>
       </c>
       <c r="AR33" s="30"/>
       <c r="AS33" s="30"/>
@@ -5309,19 +5309,19 @@
         <v>4.9189043443996</v>
       </c>
       <c r="AM34" s="89">
-        <v>5.0760141491597E-5</v>
+        <v>4.1318796492956E-5</v>
       </c>
       <c r="AN34" s="89">
         <v>7.1536562959686</v>
       </c>
       <c r="AO34" s="89">
-        <v>7.3821440780619E-5</v>
+        <v>6.0090712886137E-5</v>
       </c>
       <c r="AP34" s="89">
         <v>12.1716091518</v>
       </c>
       <c r="AQ34" s="89">
-        <v>0.00012560370348109</v>
+        <v>0.00010224151687512</v>
       </c>
       <c r="AR34" s="30"/>
       <c r="AS34" s="30"/>
@@ -5457,19 +5457,19 @@
         <v>0.080832841231858</v>
       </c>
       <c r="AM35" s="90">
-        <v>3.5034149715938E-10</v>
+        <v>2.85178263866E-10</v>
       </c>
       <c r="AN35" s="90">
         <v>0.66141093839704</v>
       </c>
       <c r="AO35" s="90">
-        <v>2.8666528958317E-9</v>
+        <v>2.3334577906648E-9</v>
       </c>
       <c r="AP35" s="90">
         <v>0.72834582851901</v>
       </c>
       <c r="AQ35" s="90">
-        <v>3.156758615984E-9</v>
+        <v>2.5696040830151E-9</v>
       </c>
       <c r="AR35" s="36"/>
       <c r="AS35" s="36"/>
@@ -5601,19 +5601,19 @@
         <v>13.463464942479</v>
       </c>
       <c r="AM36" s="89">
-        <v>5.8352649653515E-8</v>
+        <v>4.7499104317065E-8</v>
       </c>
       <c r="AN36" s="89">
         <v>2.7007728124021</v>
       </c>
       <c r="AO36" s="89">
-        <v>1.1705549083327E-8</v>
+        <v>9.5283264821546E-9</v>
       </c>
       <c r="AP36" s="89">
         <v>16.917205123089</v>
       </c>
       <c r="AQ36" s="89">
-        <v>7.3321670749826E-8</v>
+        <v>5.9683899674258E-8</v>
       </c>
       <c r="AR36" s="30"/>
       <c r="AS36" s="30"/>
@@ -6036,19 +6036,19 @@
         <v>82.051926543062</v>
       </c>
       <c r="AM39" s="89">
-        <v>3.5562519332276E-7</v>
+        <v>2.8947919684392E-7</v>
       </c>
       <c r="AN39" s="89">
         <v>364.78111157289</v>
       </c>
       <c r="AO39" s="89">
-        <v>1.5810153251614E-6</v>
+        <v>1.2869477616291E-6</v>
       </c>
       <c r="AP39" s="89">
         <v>441.47825895623</v>
       </c>
       <c r="AQ39" s="89">
-        <v>1.9134321130986E-6</v>
+        <v>1.5575352975976E-6</v>
       </c>
       <c r="AR39" s="30"/>
       <c r="AS39" s="30"/>
@@ -6181,19 +6181,19 @@
         <v>120.67515632653</v>
       </c>
       <c r="AM40" s="89">
-        <v>5.2302398744231E-7</v>
+        <v>4.2574195151999E-7</v>
       </c>
       <c r="AN40" s="89">
         <v>462.52806748284</v>
       </c>
       <c r="AO40" s="89">
-        <v>2.0046650986246E-6</v>
+        <v>1.6317990220795E-6</v>
       </c>
       <c r="AP40" s="89">
         <v>577.4392735328</v>
       </c>
       <c r="AQ40" s="89">
-        <v>2.5027072725036E-6</v>
+        <v>2.0372057570237E-6</v>
       </c>
       <c r="AR40" s="30"/>
       <c r="AS40" s="30"/>
@@ -6324,7 +6324,7 @@
         <v>0.60624630923894</v>
       </c>
       <c r="AM41" s="89">
-        <v>2.6275612286953E-9</v>
+        <v>2.138836978995E-9</v>
       </c>
       <c r="AN41" s="89">
         <v>0</v>
@@ -6336,7 +6336,7 @@
         <v>0.64362341173126</v>
       </c>
       <c r="AQ41" s="89">
-        <v>2.7895591227082E-9</v>
+        <v>2.2707033965879E-9</v>
       </c>
       <c r="AR41" s="30"/>
       <c r="AS41" s="30"/>
@@ -6466,7 +6466,7 @@
         <v>0.30312315461947</v>
       </c>
       <c r="AM42" s="89">
-        <v>1.3137806143477E-9</v>
+        <v>1.0694184894975E-9</v>
       </c>
       <c r="AN42" s="89">
         <v>0</v>
@@ -6478,7 +6478,7 @@
         <v>0.32181170586563</v>
       </c>
       <c r="AQ42" s="89">
-        <v>1.3947795613541E-9</v>
+        <v>1.1353516982939E-9</v>
       </c>
       <c r="AR42" s="30"/>
       <c r="AS42" s="30"/>
@@ -6614,19 +6614,19 @@
         <v>11.08241641518</v>
       </c>
       <c r="AM43" s="89">
-        <v>4.8032832941019E-8</v>
+        <v>3.9098765112755E-8</v>
       </c>
       <c r="AN43" s="89">
         <v>19.615194830816</v>
       </c>
       <c r="AO43" s="89">
-        <v>8.5015157445592E-8</v>
+        <v>6.9202407363119E-8</v>
       </c>
       <c r="AP43" s="89">
         <v>30.820916222421</v>
       </c>
       <c r="AQ43" s="89">
-        <v>1.3358241240357E-7</v>
+        <v>1.087361924327E-7</v>
       </c>
       <c r="AR43" s="30"/>
       <c r="AS43" s="30"/>
@@ -6758,19 +6758,19 @@
         <v>10.81676965956</v>
       </c>
       <c r="AM44" s="89">
-        <v>4.6881480586442E-8</v>
+        <v>3.8161563358927E-8</v>
       </c>
       <c r="AN44" s="89">
         <v>36.446206785644</v>
       </c>
       <c r="AO44" s="89">
-        <v>1.5796325424758E-7</v>
+        <v>1.2858221753975E-7</v>
       </c>
       <c r="AP44" s="89">
         <v>46.889421729638</v>
       </c>
       <c r="AQ44" s="89">
-        <v>2.0322569341067E-7</v>
+        <v>1.6542587986216E-7</v>
       </c>
       <c r="AR44" s="30"/>
       <c r="AS44" s="30"/>
@@ -7190,19 +7190,19 @@
         <v>0.60740684408759</v>
       </c>
       <c r="AM47" s="89">
-        <v>2.6325911584885E-9</v>
+        <v>2.142931345941E-9</v>
       </c>
       <c r="AN47" s="89">
         <v>17.479434066522</v>
       </c>
       <c r="AO47" s="89">
-        <v>7.575845420055E-8</v>
+        <v>6.1667443386691E-8</v>
       </c>
       <c r="AP47" s="89">
         <v>17.625297110976</v>
       </c>
       <c r="AQ47" s="89">
-        <v>7.6390646222941E-8</v>
+        <v>6.2182048207522E-8</v>
       </c>
       <c r="AR47" s="30"/>
       <c r="AS47" s="30"/>
@@ -7334,19 +7334,19 @@
         <v>1.1743198985693</v>
       </c>
       <c r="AM48" s="89">
-        <v>5.0896762397445E-9</v>
+        <v>4.1430006021526E-9</v>
       </c>
       <c r="AN48" s="89">
         <v>3.2001489136941</v>
       </c>
       <c r="AO48" s="89">
-        <v>1.386991901399E-8</v>
+        <v>1.1290125367513E-8</v>
       </c>
       <c r="AP48" s="89">
         <v>4.3555136005162</v>
       </c>
       <c r="AQ48" s="89">
-        <v>1.887744056065E-8</v>
+        <v>1.5366251982621E-8</v>
       </c>
       <c r="AR48" s="30"/>
       <c r="AS48" s="30"/>
@@ -7624,13 +7624,13 @@
         <v>1.9862993257412</v>
       </c>
       <c r="AO50" s="89">
-        <v>8.6089152500625E-9</v>
+        <v>7.0076640212149E-9</v>
       </c>
       <c r="AP50" s="89">
         <v>1.9295956379046</v>
       </c>
       <c r="AQ50" s="89">
-        <v>8.3631530748328E-9</v>
+        <v>6.8076134105273E-9</v>
       </c>
       <c r="AR50" s="30"/>
       <c r="AS50" s="30"/>
@@ -7766,19 +7766,19 @@
         <v>0.2024689480292</v>
       </c>
       <c r="AM51" s="89">
-        <v>8.7753038616285E-10</v>
+        <v>7.1431044864701E-10</v>
       </c>
       <c r="AN51" s="89">
         <v>11.421211768437</v>
       </c>
       <c r="AO51" s="89">
-        <v>4.9501222143749E-8</v>
+        <v>4.0294035119047E-8</v>
       </c>
       <c r="AP51" s="89">
         <v>11.310117662897</v>
       </c>
       <c r="AQ51" s="89">
-        <v>4.9019723848411E-8</v>
+        <v>3.9902095114702E-8</v>
       </c>
       <c r="AR51" s="30"/>
       <c r="AS51" s="30"/>
@@ -7910,19 +7910,19 @@
         <v>0.16166568246372</v>
       </c>
       <c r="AM52" s="89">
-        <v>7.0068299431875E-10</v>
+        <v>5.7035652773199E-10</v>
       </c>
       <c r="AN52" s="89">
         <v>0.24254030530725</v>
       </c>
       <c r="AO52" s="89">
-        <v>1.0512055791668E-9</v>
+        <v>8.5568219712397E-10</v>
       </c>
       <c r="AP52" s="89">
         <v>0.40724931920111</v>
       </c>
       <c r="AQ52" s="89">
-        <v>1.7650788223169E-9</v>
+        <v>1.4367755981415E-9</v>
       </c>
       <c r="AR52" s="30"/>
       <c r="AS52" s="30"/>

</xml_diff>